<commit_message>
Implémentation du server et du client-test Webservice.
</commit_message>
<xml_diff>
--- a/doc/2014/AconitBacklog.xlsx
+++ b/doc/2014/AconitBacklog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="300" windowWidth="13935" windowHeight="8370" tabRatio="824" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="300" windowWidth="13935" windowHeight="8370" tabRatio="824" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Accueil" sheetId="1" r:id="rId1"/>
@@ -5083,15 +5083,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>79945</xdr:colOff>
+      <xdr:colOff>44226</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>102053</xdr:rowOff>
+      <xdr:rowOff>90147</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>426927</xdr:colOff>
+      <xdr:colOff>391208</xdr:colOff>
       <xdr:row>76</xdr:row>
-      <xdr:rowOff>102053</xdr:rowOff>
+      <xdr:rowOff>90147</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -23863,8 +23863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AG32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -24526,7 +24526,7 @@
   <dimension ref="A1:O158"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H65" sqref="H65"/>
     </sheetView>
   </sheetViews>
@@ -30703,8 +30703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:CE55"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="F21" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AE60" sqref="AE60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
maj charges dispo backlog
</commit_message>
<xml_diff>
--- a/doc/2014/AconitBacklog.xlsx
+++ b/doc/2014/AconitBacklog.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="211">
   <si>
     <t>Rédacteur</t>
   </si>
@@ -688,6 +688,9 @@
   </si>
   <si>
     <t>Gestion des utilisateurs autorisés</t>
+  </si>
+  <si>
+    <t>Badin</t>
   </si>
 </sst>
 </file>
@@ -2574,7 +2577,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout>
@@ -2722,11 +2724,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="122132352"/>
-        <c:axId val="122133888"/>
+        <c:axId val="120436608"/>
+        <c:axId val="120438144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="122132352"/>
+        <c:axId val="120436608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2734,14 +2736,14 @@
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122133888"/>
+        <c:crossAx val="120438144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="122133888"/>
+        <c:axId val="120438144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2755,21 +2757,20 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="122132352"/>
+        <c:crossAx val="120436608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000899" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000899" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000921" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000921" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2795,7 +2796,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3105,11 +3105,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="122909440"/>
-        <c:axId val="122910976"/>
+        <c:axId val="123233024"/>
+        <c:axId val="123234560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="122909440"/>
+        <c:axId val="123233024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3117,14 +3117,14 @@
         <c:numFmt formatCode="dd/mm" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122910976"/>
+        <c:crossAx val="123234560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="122910976"/>
+        <c:axId val="123234560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3138,21 +3138,20 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="122909440"/>
+        <c:crossAx val="123233024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000921" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000921" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000944" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000944" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3178,7 +3177,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3469,11 +3467,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="122817536"/>
-        <c:axId val="122839808"/>
+        <c:axId val="123354112"/>
+        <c:axId val="123384576"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="122817536"/>
+        <c:axId val="123354112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3481,14 +3479,14 @@
         <c:numFmt formatCode="dd/mm" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122839808"/>
+        <c:crossAx val="123384576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="122839808"/>
+        <c:axId val="123384576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3502,21 +3500,20 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="122817536"/>
+        <c:crossAx val="123354112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000944" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000944" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000966" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000966" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3542,7 +3539,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3915,11 +3911,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="123254272"/>
-        <c:axId val="123255808"/>
+        <c:axId val="123549184"/>
+        <c:axId val="123550720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="123254272"/>
+        <c:axId val="123549184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3927,14 +3923,14 @@
         <c:numFmt formatCode="dd/mm" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123255808"/>
+        <c:crossAx val="123550720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="123255808"/>
+        <c:axId val="123550720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3948,21 +3944,20 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="123254272"/>
+        <c:crossAx val="123549184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000966" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000966" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000988" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000988" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3988,7 +3983,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -4361,11 +4355,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="123284864"/>
-        <c:axId val="123556992"/>
+        <c:axId val="123559296"/>
+        <c:axId val="123831424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="123284864"/>
+        <c:axId val="123559296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4373,14 +4367,14 @@
         <c:numFmt formatCode="dd/mm" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123556992"/>
+        <c:crossAx val="123831424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="123556992"/>
+        <c:axId val="123831424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4394,21 +4388,20 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="123284864"/>
+        <c:crossAx val="123559296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000988" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000988" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.7500000000000101" l="0.70000000000000062" r="0.70000000000000062" t="0.7500000000000101" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -12066,7 +12059,7 @@
       <selection activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="E3" sqref="E3"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="H19" sqref="H19"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -21067,80 +21060,228 @@
       <c r="NE11" s="146"/>
     </row>
     <row r="12" spans="1:379" s="147" customFormat="1">
-      <c r="A12" s="145"/>
-      <c r="B12" s="145"/>
-      <c r="C12" s="145"/>
-      <c r="D12" s="145"/>
-      <c r="E12" s="146"/>
-      <c r="F12" s="146"/>
-      <c r="G12" s="146"/>
-      <c r="H12" s="146"/>
-      <c r="I12" s="146"/>
-      <c r="J12" s="146"/>
-      <c r="K12" s="146"/>
-      <c r="L12" s="146"/>
-      <c r="M12" s="146"/>
-      <c r="N12" s="146"/>
-      <c r="O12" s="146"/>
-      <c r="P12" s="146"/>
-      <c r="Q12" s="146"/>
-      <c r="R12" s="146"/>
-      <c r="S12" s="146"/>
-      <c r="T12" s="146"/>
-      <c r="U12" s="146"/>
-      <c r="V12" s="146"/>
-      <c r="W12" s="146"/>
-      <c r="X12" s="146"/>
-      <c r="Y12" s="146"/>
-      <c r="Z12" s="146"/>
-      <c r="AA12" s="146"/>
-      <c r="AB12" s="146"/>
-      <c r="AC12" s="146"/>
-      <c r="AD12" s="146"/>
-      <c r="AE12" s="146"/>
-      <c r="AF12" s="146"/>
-      <c r="AG12" s="146"/>
-      <c r="AH12" s="146"/>
-      <c r="AI12" s="146"/>
-      <c r="AJ12" s="146"/>
-      <c r="AK12" s="146"/>
-      <c r="AL12" s="146"/>
-      <c r="AM12" s="146"/>
-      <c r="AN12" s="146"/>
-      <c r="AO12" s="146"/>
-      <c r="AP12" s="146"/>
-      <c r="AQ12" s="146"/>
-      <c r="AR12" s="146"/>
-      <c r="AS12" s="146"/>
-      <c r="AT12" s="146"/>
-      <c r="AU12" s="146"/>
-      <c r="AV12" s="146"/>
-      <c r="AW12" s="146"/>
-      <c r="AX12" s="146"/>
-      <c r="AY12" s="146"/>
-      <c r="AZ12" s="146"/>
-      <c r="BA12" s="146"/>
-      <c r="BB12" s="146"/>
-      <c r="BC12" s="146"/>
-      <c r="BD12" s="146"/>
-      <c r="BE12" s="146"/>
-      <c r="BF12" s="146"/>
-      <c r="BG12" s="146"/>
-      <c r="BH12" s="146"/>
-      <c r="BI12" s="146"/>
-      <c r="BJ12" s="146"/>
-      <c r="BK12" s="146"/>
-      <c r="BL12" s="146"/>
-      <c r="BM12" s="146"/>
-      <c r="BN12" s="146"/>
-      <c r="BO12" s="146"/>
-      <c r="BP12" s="146"/>
-      <c r="BQ12" s="146"/>
-      <c r="BR12" s="146"/>
-      <c r="BS12" s="146"/>
-      <c r="BT12" s="146"/>
-      <c r="BU12" s="146"/>
-      <c r="BV12" s="146"/>
+      <c r="A12" s="145" t="s">
+        <v>210</v>
+      </c>
+      <c r="B12" s="145" t="s">
+        <v>204</v>
+      </c>
+      <c r="C12" s="145" t="s">
+        <v>193</v>
+      </c>
+      <c r="D12" s="145" t="s">
+        <v>194</v>
+      </c>
+      <c r="E12" s="146">
+        <v>1</v>
+      </c>
+      <c r="F12" s="146">
+        <v>1</v>
+      </c>
+      <c r="G12" s="146">
+        <v>1</v>
+      </c>
+      <c r="H12" s="146">
+        <v>1</v>
+      </c>
+      <c r="I12" s="146">
+        <v>1</v>
+      </c>
+      <c r="J12" s="146">
+        <v>1</v>
+      </c>
+      <c r="K12" s="146">
+        <v>1</v>
+      </c>
+      <c r="L12" s="146">
+        <v>1</v>
+      </c>
+      <c r="M12" s="146">
+        <v>1</v>
+      </c>
+      <c r="N12" s="146">
+        <v>1</v>
+      </c>
+      <c r="O12" s="146">
+        <v>1</v>
+      </c>
+      <c r="P12" s="146">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="146">
+        <v>1</v>
+      </c>
+      <c r="R12" s="146">
+        <v>1</v>
+      </c>
+      <c r="S12" s="146">
+        <v>1</v>
+      </c>
+      <c r="T12" s="146">
+        <v>1</v>
+      </c>
+      <c r="U12" s="146">
+        <v>1</v>
+      </c>
+      <c r="V12" s="146">
+        <v>1</v>
+      </c>
+      <c r="W12" s="146">
+        <v>1</v>
+      </c>
+      <c r="X12" s="146">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="146">
+        <v>1</v>
+      </c>
+      <c r="Z12" s="146">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="146">
+        <v>1</v>
+      </c>
+      <c r="AB12" s="146">
+        <v>1</v>
+      </c>
+      <c r="AC12" s="146">
+        <v>1</v>
+      </c>
+      <c r="AD12" s="146">
+        <v>1</v>
+      </c>
+      <c r="AE12" s="146">
+        <v>1</v>
+      </c>
+      <c r="AF12" s="146">
+        <v>1</v>
+      </c>
+      <c r="AG12" s="146">
+        <v>1</v>
+      </c>
+      <c r="AH12" s="146">
+        <v>1</v>
+      </c>
+      <c r="AI12" s="146">
+        <v>0</v>
+      </c>
+      <c r="AJ12" s="146">
+        <v>1</v>
+      </c>
+      <c r="AK12" s="146">
+        <v>1</v>
+      </c>
+      <c r="AL12" s="146">
+        <v>1</v>
+      </c>
+      <c r="AM12" s="146">
+        <v>1</v>
+      </c>
+      <c r="AN12" s="146">
+        <v>1</v>
+      </c>
+      <c r="AO12" s="146">
+        <v>1</v>
+      </c>
+      <c r="AP12" s="146">
+        <v>1</v>
+      </c>
+      <c r="AQ12" s="146">
+        <v>1</v>
+      </c>
+      <c r="AR12" s="146">
+        <v>1</v>
+      </c>
+      <c r="AS12" s="146">
+        <v>1</v>
+      </c>
+      <c r="AT12" s="146">
+        <v>1</v>
+      </c>
+      <c r="AU12" s="146">
+        <v>1</v>
+      </c>
+      <c r="AV12" s="146">
+        <v>1</v>
+      </c>
+      <c r="AW12" s="146">
+        <v>1</v>
+      </c>
+      <c r="AX12" s="146">
+        <v>1</v>
+      </c>
+      <c r="AY12" s="146">
+        <v>1</v>
+      </c>
+      <c r="AZ12" s="146">
+        <v>1</v>
+      </c>
+      <c r="BA12" s="146">
+        <v>1</v>
+      </c>
+      <c r="BB12" s="146">
+        <v>1</v>
+      </c>
+      <c r="BC12" s="146">
+        <v>1</v>
+      </c>
+      <c r="BD12" s="146">
+        <v>1</v>
+      </c>
+      <c r="BE12" s="146">
+        <v>1</v>
+      </c>
+      <c r="BF12" s="146">
+        <v>1</v>
+      </c>
+      <c r="BG12" s="146">
+        <v>0</v>
+      </c>
+      <c r="BH12" s="146">
+        <v>1</v>
+      </c>
+      <c r="BI12" s="146">
+        <v>1</v>
+      </c>
+      <c r="BJ12" s="146">
+        <v>1</v>
+      </c>
+      <c r="BK12" s="146">
+        <v>1</v>
+      </c>
+      <c r="BL12" s="146">
+        <v>1</v>
+      </c>
+      <c r="BM12" s="146">
+        <v>1</v>
+      </c>
+      <c r="BN12" s="146">
+        <v>1</v>
+      </c>
+      <c r="BO12" s="146">
+        <v>1</v>
+      </c>
+      <c r="BP12" s="146">
+        <v>1</v>
+      </c>
+      <c r="BQ12" s="146">
+        <v>1</v>
+      </c>
+      <c r="BR12" s="146">
+        <v>1</v>
+      </c>
+      <c r="BS12" s="146">
+        <v>1</v>
+      </c>
+      <c r="BT12" s="146">
+        <v>1</v>
+      </c>
+      <c r="BU12" s="146">
+        <v>1</v>
+      </c>
+      <c r="BV12" s="146">
+        <v>1</v>
+      </c>
       <c r="BW12" s="146"/>
       <c r="BX12" s="146"/>
       <c r="BY12" s="146"/>
@@ -23399,7 +23540,7 @@
   <dimension ref="A1:AG41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -23533,7 +23674,7 @@
       </c>
       <c r="I7" s="15">
         <f ca="1">IF($AD7,SUM(INDIRECT(AG7)),"")</f>
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="J7" s="22">
         <v>0</v>
@@ -23592,7 +23733,7 @@
       </c>
       <c r="I8" s="15">
         <f t="shared" ref="I8:I11" ca="1" si="6">IF($AD8,SUM(INDIRECT(AG8)),"")</f>
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="J8" s="22">
         <v>0</v>
@@ -23651,7 +23792,7 @@
       </c>
       <c r="I9" s="15">
         <f t="shared" ca="1" si="6"/>
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="J9" s="22">
         <v>0</v>
@@ -23711,7 +23852,7 @@
       </c>
       <c r="I10" s="15">
         <f t="shared" ca="1" si="6"/>
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="J10" s="22">
         <v>0</v>
@@ -23771,7 +23912,7 @@
       </c>
       <c r="I11" s="15">
         <f t="shared" ca="1" si="6"/>
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="J11" s="22">
         <v>0</v>
@@ -23817,7 +23958,7 @@
       </c>
       <c r="I12" s="108">
         <f ca="1">SUM(I7:I11)</f>
-        <v>312</v>
+        <v>380</v>
       </c>
       <c r="J12" s="110">
         <f>AVERAGE(J7:J11)</f>
@@ -38438,7 +38579,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:83">
+    <row r="9" spans="1:83" ht="25.5">
       <c r="A9" s="90">
         <f t="shared" ca="1" si="17"/>
         <v>21</v>
@@ -51446,7 +51587,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:83">
+    <row r="13" spans="1:83" ht="25.5">
       <c r="A13" s="90">
         <f t="shared" ca="1" si="17"/>
         <v>76</v>

</xml_diff>